<commit_message>
Ajout des problèmes dans l'outil d'importation.
</commit_message>
<xml_diff>
--- a/OutilImportation/OutilImportation/Data/problems_3.xlsx
+++ b/OutilImportation/OutilImportation/Data/problems_3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\Documents\Cegep\Projet\GreenHouse-Tech\OutilImportation\OutilImportation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124CF069-B0CA-4829-B861-8F9305E6591F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -113,18 +114,12 @@
     <t>Maladies cryptogamiques</t>
   </si>
   <si>
-    <t>Diminuer le taux d'humidité général , Diluer 1 cuillère à soupe de bicarbonate dans 1 litre d'eau (idéalement de l'eau de pluie ou de l'eau minérale qui est moins calcaire), Par temps sec, pulvériser cette solution sur toutes les feuilles en prenant soin de bien atteindre le dessus et le dessous des feuilles.</t>
-  </si>
-  <si>
     <t>Mauvaises herbes</t>
   </si>
   <si>
     <t>Plante nocive</t>
   </si>
   <si>
-    <t>Cueillette manuelle ou Ajoutez dans un litre d'eau, 250 grammes de bicarbonate de soude et 50 ml de vinaigre blanc. Faites bien attention à respecter ce dosage pour ne pas acidifier votre sol. Mélangez le tout dans un pulvérisateur, et arrosez les adventices de cette potion.</t>
-  </si>
-  <si>
     <t>Aération</t>
   </si>
   <si>
@@ -153,12 +148,18 @@
   </si>
   <si>
     <t>1,2,4,5,6,8,15,16,18,19</t>
+  </si>
+  <si>
+    <t>Cueillette manuelle ou Ajoutez dans un litre d'eau, 250 grammes de bicarbonate de soude et 50 ml de vinaigre blanc. Mélangez le tout dans un pulvérisateur, et arrosez les adventices de cette potion.</t>
+  </si>
+  <si>
+    <t>Diminuer le taux d'humidité général , Diluer 1 cuillère à soupe de bicarbonate dans 1 litre d'eau, Par temps sec, pulvériser cette solution sur toutes les feuilles en prenant soin de bien atteindre le dessus et le dessous des feuilles.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,6 +242,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,19 +525,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -544,11 +548,11 @@
         <v>17</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -559,11 +563,11 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -574,11 +578,11 @@
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -589,11 +593,11 @@
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -604,11 +608,11 @@
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -619,11 +623,11 @@
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -634,11 +638,11 @@
         <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -653,7 +657,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -664,11 +668,11 @@
         <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -679,11 +683,11 @@
         <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -694,11 +698,11 @@
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -713,7 +717,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -724,11 +728,11 @@
         <v>20</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -739,50 +743,50 @@
         <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1010,13 +1014,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E8645F3-BD5D-4315-9CDD-32119245D3D3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E8645F3-BD5D-4315-9CDD-32119245D3D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7a2aa5ce-9268-4b11-b8eb-4b0ce9691849"/>
+    <ds:schemaRef ds:uri="705fa277-30ce-4e89-832c-36cb769920f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58E3C05D-4530-421A-B52D-10A61AE8016D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58E3C05D-4530-421A-B52D-10A61AE8016D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB0115ED-6644-41B3-9829-73291665D3FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB0115ED-6644-41B3-9829-73291665D3FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>